<commit_message>
Added some pics and updated spreadsheet
</commit_message>
<xml_diff>
--- a/.Notes/leves.xlsx
+++ b/.Notes/leves.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Steam\Steam\steamapps\common\Stardew Valley\SiMods\[Si]\CBLeaves\.Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38911C2E-EA92-4C8C-AB18-6669CE547553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C267F300-3588-443A-86A4-C2859741A1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
   <si>
     <t>Leaf</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Tea leaves</t>
   </si>
   <si>
-    <t>Those big pink trees randomly around; cherry blossoms?</t>
-  </si>
-  <si>
     <t>Prize for getting them all: hat that is just some leaves strewn on top of our head lol</t>
   </si>
   <si>
@@ -248,10 +245,64 @@
     <t>Money tree?</t>
   </si>
   <si>
-    <t>Larimar/amber tree?</t>
-  </si>
-  <si>
     <t>RSV</t>
+  </si>
+  <si>
+    <t>4 seasons</t>
+  </si>
+  <si>
+    <t>3 seasons</t>
+  </si>
+  <si>
+    <t>Larimar</t>
+  </si>
+  <si>
+    <t>Amber</t>
+  </si>
+  <si>
+    <t>1 season</t>
+  </si>
+  <si>
+    <t>Casolatier</t>
+  </si>
+  <si>
+    <t>Trellis grape</t>
+  </si>
+  <si>
+    <t>Those big pink trees randomly around; cherry blossoms? 1 week per Spring</t>
+  </si>
+  <si>
+    <t>Cherry pluot</t>
+  </si>
+  <si>
+    <t>Mtn plumcot</t>
+  </si>
+  <si>
+    <t>Desert tangelo</t>
+  </si>
+  <si>
+    <t>Paradise rangpur</t>
+  </si>
+  <si>
+    <t>Tropi ugli</t>
+  </si>
+  <si>
+    <t>Ember blood lime</t>
+  </si>
+  <si>
+    <t>Highland jostaberry</t>
+  </si>
+  <si>
+    <t>North limequat</t>
+  </si>
+  <si>
+    <t>Nevaril bush</t>
+  </si>
+  <si>
+    <t>Rosemary bush</t>
+  </si>
+  <si>
+    <t>Sea buckthorn bush</t>
   </si>
 </sst>
 </file>
@@ -592,11 +643,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,7 +730,7 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -687,7 +738,7 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -738,10 +789,10 @@
       </c>
       <c r="B16" s="3"/>
       <c r="D16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>39</v>
       </c>
@@ -752,16 +803,25 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
-      </c>
-      <c r="J17" t="s">
-        <v>64</v>
-      </c>
-      <c r="N17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="G17">
+        <v>24</v>
+      </c>
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17">
+        <v>20</v>
+      </c>
+      <c r="L17" t="s">
+        <v>69</v>
+      </c>
+      <c r="M17">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>32</v>
       </c>
@@ -769,13 +829,25 @@
         <v>34</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="G18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" t="s">
+        <v>64</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="L18" t="s">
+        <v>78</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>23</v>
       </c>
@@ -783,13 +855,25 @@
         <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" t="s">
+        <v>65</v>
       </c>
       <c r="J19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="L19" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
@@ -797,13 +881,25 @@
         <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="G20" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" t="s">
+        <v>66</v>
       </c>
       <c r="J20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="L20" t="s">
+        <v>80</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -814,13 +910,25 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="G21" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" t="s">
+        <v>67</v>
       </c>
       <c r="J21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="L21" t="s">
+        <v>81</v>
+      </c>
+      <c r="M21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
@@ -828,29 +936,71 @@
         <v>4</v>
       </c>
       <c r="F22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" t="s">
         <v>70</v>
       </c>
-      <c r="J22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L22" t="s">
+        <v>82</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" t="s">
+        <v>62</v>
+      </c>
+      <c r="J23" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" t="s">
+        <v>83</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L24" t="s">
+        <v>84</v>
+      </c>
+      <c r="M24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>41</v>
       </c>
@@ -858,42 +1008,72 @@
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="F25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" t="s">
+        <v>74</v>
+      </c>
+      <c r="L25" t="s">
+        <v>85</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>44</v>
       </c>
@@ -901,10 +1081,10 @@
         <v>45</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -912,7 +1092,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>5</v>
       </c>
@@ -1056,7 +1236,7 @@
         <v>51</v>
       </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>